<commit_message>
Changed csv to tsv
</commit_message>
<xml_diff>
--- a/src/resources/vragen.xlsx
+++ b/src/resources/vragen.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Table 1</t>
   </si>
@@ -37,37 +37,58 @@
     <t>Cardio is goed?</t>
   </si>
   <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
     <t>Extra informatie over cardio…</t>
   </si>
   <si>
-    <t>vraag1-plaatje.jpg</t>
+    <t>vraag1-plaatje.jpeg</t>
   </si>
   <si>
     <t>Zie je huid er mooi bruin uit?</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
     <t>Extra informatie over je huid…</t>
   </si>
   <si>
-    <t>vraag2-plaatje.jpg</t>
+    <t>vraag2-plaatje.jpeg</t>
   </si>
   <si>
     <t>Ben je kaal?</t>
   </si>
   <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
     <t>Extra informatie over je haarlijn…</t>
   </si>
   <si>
-    <t>vraag3-plaatje.jpg</t>
-  </si>
-  <si>
-    <t>Heb je een lekker buikje?</t>
+    <t>vraag3-plaatje.jpeg</t>
+  </si>
+  <si>
+    <t>Heb je een lekker pokkeltje?</t>
+  </si>
+  <si>
+    <t>C3</t>
   </si>
   <si>
     <t>Extra informatie over je vet…</t>
   </si>
   <si>
-    <t>vraag4-plaatje.jpg</t>
+    <t>vraag4-plaatje.jpeg</t>
   </si>
   <si>
     <t>Voelt je middenvoetsbeentje goed?</t>
@@ -76,7 +97,7 @@
     <t>Extra informatie over je middenvoetsbeentje…</t>
   </si>
   <si>
-    <t>vraag5-plaatje.jpg</t>
+    <t>vraag5-plaatje.jpeg</t>
   </si>
 </sst>
 </file>
@@ -265,6 +286,9 @@
     <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -272,9 +296,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1362,7 +1383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1370,8 +1391,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1384,6 +1405,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" s="3"/>
@@ -1393,6 +1415,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" s="4"/>
@@ -1414,238 +1437,271 @@
       <c r="G3" t="s" s="6">
         <v>6</v>
       </c>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" ht="32.05" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="E4" s="10">
+      <c r="C5" t="s" s="10">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="F4" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10">
+      <c r="C6" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" ht="32.05" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="F5" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s" s="9">
+      <c r="C7" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E7" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" ht="56.05" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" ht="32.05" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" ht="56.05" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s" s="9">
+      <c r="C8" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s" s="9">
-        <v>21</v>
-      </c>
+      <c r="F8" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="12"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="12"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="12"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="12"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="12"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="12"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="12"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="12"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="7"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="12"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="7"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="12"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="7"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="12"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="7"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="12"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="7"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="12"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="12"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="7"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="12"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>